<commit_message>
Update code with Dataprovider Add test with data from Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>city</t>
   </si>
@@ -27,10 +27,13 @@
     <t>Dubai</t>
   </si>
   <si>
-    <t>xxx</t>
-  </si>
-  <si>
     <t>London</t>
+  </si>
+  <si>
+    <t>Jumeirah Beach Hotel</t>
+  </si>
+  <si>
+    <t>Grand Plaza Apartments</t>
   </si>
 </sst>
 </file>
@@ -366,7 +369,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -387,15 +390,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>